<commit_message>
added questions 1-7 to word file
</commit_message>
<xml_diff>
--- a/pred400/week2/nwspa_hw2_linearsystem.xlsx
+++ b/pred400/week2/nwspa_hw2_linearsystem.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\nwspa\pred400\week2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="28755" windowHeight="13095"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="28752" windowHeight="13092"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>total hires</t>
   </si>
@@ -34,13 +39,34 @@
   </si>
   <si>
     <t>campus 3 is required to hire 100</t>
+  </si>
+  <si>
+    <t>Append the RHS to the matrix</t>
+  </si>
+  <si>
+    <t>add row1 to row2</t>
+  </si>
+  <si>
+    <t>divide row2 by 2 to get a 1 in its pivot location</t>
+  </si>
+  <si>
+    <t>subtract row2 from row1</t>
+  </si>
+  <si>
+    <t>subtract row 3 from row2</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>mmult(C4:E6, F26:27) = G4:G6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,12 +75,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,14 +101,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -123,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -155,9 +197,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,6 +232,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -364,120 +408,394 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C6:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="6" spans="3:8">
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:8">
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>300</v>
       </c>
-      <c r="H7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8">
-      <c r="C8">
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="1">
         <v>-1</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="3:8">
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
         <v>100</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="3:8">
-      <c r="C11">
-        <f t="array" ref="C11:E13">MINVERSE(C7:E9)</f>
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>-0.5</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f t="array" ref="G11:G13">MMULT(C11:E13,G7:G9)</f>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>300</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>100</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>300</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>300</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>100</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="1">
+        <f t="array" ref="C16:F16">C12:F12</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>300</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C17" s="1">
+        <f t="array" ref="C17:F17">C13:F13/2</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="3:8">
-      <c r="C12">
-        <v>0.5</v>
-      </c>
-      <c r="D12">
-        <v>0.5</v>
-      </c>
-      <c r="E12">
-        <v>-1</v>
-      </c>
-      <c r="G12">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="1">
+        <f t="array" ref="C18:F18">C14:F14</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <f t="array" ref="C21:F21">C12:F12-C17:F17</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>150</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C22" s="1">
+        <f t="array" ref="C22:F22">C17:F17</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>150</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
+        <f t="array" ref="C23:F23">C18:F18</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>100</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="N24" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25">
+        <f t="array" ref="N25:N27">MMULT(C4:E6,F26:F28)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <f t="array" ref="C26:F26">C21:F21</f>
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>150</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <f t="array" ref="C27:F27">C22:F22-C23:F23</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="3:8">
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="N27">
         <v>100</v>
       </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <f t="array" ref="C28:F28">C23:F23</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>100</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -485,24 +803,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>